<commit_message>
Generate graphs of accuracy and loss
</commit_message>
<xml_diff>
--- a/outputs/cnn_spec_results.xlsx
+++ b/outputs/cnn_spec_results.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2374999970197678</v>
+        <v>0.2249999940395355</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1966799050569534</v>
+        <v>0.2156264036893845</v>
       </c>
       <c r="D2" t="n">
         <v>0.2000000029802322</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1920216977596283</v>
+        <v>0.1917306184768677</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.25</v>
+        <v>0.2374999970197678</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1898896992206573</v>
+        <v>0.1901871562004089</v>
       </c>
       <c r="D3" t="n">
         <v>0.2000000029802322</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1899911463260651</v>
+        <v>0.1877334713935852</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.21875</v>
+        <v>0.3125</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1897294372320175</v>
+        <v>0.1881064027547836</v>
       </c>
       <c r="D4" t="n">
         <v>0.2000000029802322</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1910883635282516</v>
+        <v>0.1862240731716156</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2312500029802322</v>
+        <v>0.3125</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1883033812046051</v>
+        <v>0.1852631270885468</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2000000029802322</v>
+        <v>0.2249999940395355</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1925698816776276</v>
+        <v>0.1831875294446945</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2750000059604645</v>
+        <v>0.3687500059604645</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1881457716226578</v>
+        <v>0.1830499917268753</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2000000029802322</v>
+        <v>0.4000000059604645</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1897348612546921</v>
+        <v>0.1774629205465317</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.262499988079071</v>
+        <v>0.4124999940395355</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1877476871013641</v>
+        <v>0.1787919998168945</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2000000029802322</v>
+        <v>0.2249999940395355</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1914736032485962</v>
+        <v>0.1768079698085785</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.262499988079071</v>
+        <v>0.449999988079071</v>
       </c>
       <c r="C8" t="n">
-        <v>0.186520978808403</v>
+        <v>0.1716659367084503</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2000000029802322</v>
+        <v>0.4000000059604645</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1880990564823151</v>
+        <v>0.1649817228317261</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3187499940395355</v>
+        <v>0.5062500238418579</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1856988519430161</v>
+        <v>0.1633847951889038</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2750000059604645</v>
+        <v>0.625</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1833361089229584</v>
+        <v>0.1425943374633789</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.324999988079071</v>
+        <v>0.543749988079071</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1826120465993881</v>
+        <v>0.1503585129976273</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3499999940395355</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1783304810523987</v>
+        <v>0.1239223033189774</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.4000000059604645</v>
+        <v>0.6187499761581421</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1781894266605377</v>
+        <v>0.1373969167470932</v>
       </c>
       <c r="D11" t="n">
-        <v>0.625</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="E11" t="n">
-        <v>0.168193444609642</v>
+        <v>0.1063784509897232</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.425000011920929</v>
+        <v>0.637499988079071</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1715630739927292</v>
+        <v>0.1275408267974854</v>
       </c>
       <c r="D12" t="n">
-        <v>0.625</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1567563116550446</v>
+        <v>0.1056616082787514</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.518750011920929</v>
+        <v>0.6875</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1620600372552872</v>
+        <v>0.1201655119657516</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7250000238418579</v>
+        <v>0.675000011920929</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1351646482944489</v>
+        <v>0.1009130254387856</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.574999988079071</v>
+        <v>0.675000011920929</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1490680873394012</v>
+        <v>0.112513855099678</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7250000238418579</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1220766082406044</v>
+        <v>0.09546820819377899</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.574999988079071</v>
+        <v>0.71875</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1365207880735397</v>
+        <v>0.1073798313736916</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7250000238418579</v>
+        <v>0.699999988079071</v>
       </c>
       <c r="E15" t="n">
-        <v>0.09598417580127716</v>
+        <v>0.08719857037067413</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6187499761581421</v>
+        <v>0.762499988079071</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1235951334238052</v>
+        <v>0.097477987408638</v>
       </c>
       <c r="D16" t="n">
-        <v>0.75</v>
+        <v>0.7250000238418579</v>
       </c>
       <c r="E16" t="n">
-        <v>0.09499473869800568</v>
+        <v>0.08891966193914413</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6812499761581421</v>
+        <v>0.7749999761581421</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1131535395979881</v>
+        <v>0.0888277143239975</v>
       </c>
       <c r="D17" t="n">
-        <v>0.800000011920929</v>
+        <v>0.824999988079071</v>
       </c>
       <c r="E17" t="n">
-        <v>0.08132346719503403</v>
+        <v>0.07608769834041595</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.6812499761581421</v>
+        <v>0.7875000238418579</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1066324561834335</v>
+        <v>0.08468399941921234</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7250000238418579</v>
+        <v>0.800000011920929</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07931090891361237</v>
+        <v>0.07619804888963699</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7562500238418579</v>
+        <v>0.8187500238418579</v>
       </c>
       <c r="C19" t="n">
-        <v>0.09800496697425842</v>
+        <v>0.07598400861024857</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8500000238418579</v>
+        <v>0.824999988079071</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07303117960691452</v>
+        <v>0.0726330354809761</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.768750011920929</v>
+        <v>0.8125</v>
       </c>
       <c r="C20" t="n">
-        <v>0.09099246561527252</v>
+        <v>0.07229314744472504</v>
       </c>
       <c r="D20" t="n">
-        <v>0.824999988079071</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06716835498809814</v>
+        <v>0.06865433603525162</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.800000011920929</v>
+        <v>0.8812500238418579</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08085252344608307</v>
+        <v>0.06271536648273468</v>
       </c>
       <c r="D21" t="n">
-        <v>0.824999988079071</v>
+        <v>0.7749999761581421</v>
       </c>
       <c r="E21" t="n">
-        <v>0.07338474690914154</v>
+        <v>0.0709904208779335</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.824999988079071</v>
+        <v>0.8687499761581421</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07447928935289383</v>
+        <v>0.05907921120524406</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8500000238418579</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="E22" t="n">
-        <v>0.06012178212404251</v>
+        <v>0.06305022537708282</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.862500011920929</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="C23" t="n">
-        <v>0.06699880212545395</v>
+        <v>0.05201143026351929</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8500000238418579</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="E23" t="n">
-        <v>0.06102664396166801</v>
+        <v>0.06148362159729004</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.875</v>
+        <v>0.918749988079071</v>
       </c>
       <c r="C24" t="n">
-        <v>0.06244267150759697</v>
+        <v>0.04715242236852646</v>
       </c>
       <c r="D24" t="n">
-        <v>0.875</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0503539927303791</v>
+        <v>0.06075760722160339</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.887499988079071</v>
+        <v>0.9312499761581421</v>
       </c>
       <c r="C25" t="n">
-        <v>0.05464364215731621</v>
+        <v>0.04166350141167641</v>
       </c>
       <c r="D25" t="n">
-        <v>0.925000011920929</v>
+        <v>0.8500000238418579</v>
       </c>
       <c r="E25" t="n">
-        <v>0.04974279552698135</v>
+        <v>0.06533880531787872</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.925000011920929</v>
+        <v>0.9437500238418579</v>
       </c>
       <c r="C26" t="n">
-        <v>0.05020321160554886</v>
+        <v>0.03710343688726425</v>
       </c>
       <c r="D26" t="n">
-        <v>0.925000011920929</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>0.04569850116968155</v>
+        <v>0.05113442987203598</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.925000011920929</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="C27" t="n">
-        <v>0.04546488076448441</v>
+        <v>0.03333047777414322</v>
       </c>
       <c r="D27" t="n">
-        <v>0.949999988079071</v>
+        <v>0.8999999761581421</v>
       </c>
       <c r="E27" t="n">
-        <v>0.04401396960020065</v>
+        <v>0.05971075966954231</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.9375</v>
+        <v>0.981249988079071</v>
       </c>
       <c r="C28" t="n">
-        <v>0.04078754037618637</v>
+        <v>0.03051383793354034</v>
       </c>
       <c r="D28" t="n">
-        <v>0.925000011920929</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>0.04268946871161461</v>
+        <v>0.04816677421331406</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.9375</v>
+        <v>0.9750000238418579</v>
       </c>
       <c r="C29" t="n">
-        <v>0.03679747506976128</v>
+        <v>0.02773591317236423</v>
       </c>
       <c r="D29" t="n">
-        <v>0.925000011920929</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>0.04067269340157509</v>
+        <v>0.045600775629282</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.96875</v>
+        <v>0.9750000238418579</v>
       </c>
       <c r="C30" t="n">
-        <v>0.03326547890901566</v>
+        <v>0.02533054910600185</v>
       </c>
       <c r="D30" t="n">
-        <v>0.925000011920929</v>
+        <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>0.03951626643538475</v>
+        <v>0.04405773058533669</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.956250011920929</v>
+        <v>0.9750000238418579</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03174209222197533</v>
+        <v>0.02425135299563408</v>
       </c>
       <c r="D31" t="n">
-        <v>0.925000011920929</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.03754477202892303</v>
+        <v>0.0431615486741066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>